<commit_message>
Querys and smaller fixes in excel
</commit_message>
<xml_diff>
--- a/Horrific_Medusa_Excel/Address.xlsx
+++ b/Horrific_Medusa_Excel/Address.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SofiaAndersson\Documents\SCHOOL\HorrificMedusa\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BeatriceVilhelmsson\Documents\GitHubs\Projekt_HM\Horrific_Medusa_Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -13,6 +13,7 @@
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
+    <sheet name="Blad2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -552,4 +553,16 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>